<commit_message>
updated report - CM
</commit_message>
<xml_diff>
--- a/TeamACNTReport.xlsx
+++ b/TeamACNTReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10910"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tmcshea44/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/connor/Documents/ssw555/555project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1556919A-9200-8942-95FB-A5A88109B955}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C316DB7-97C9-2C47-9A0C-48E22D7BABCF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="29040" windowHeight="13960" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="13960" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -23,18 +23,10 @@
     <sheet name="Sprint4" sheetId="6" r:id="rId8"/>
     <sheet name="Stories" sheetId="11" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -44,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="219">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -698,6 +690,39 @@
   </si>
   <si>
     <t>parser.py</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>birthBeforeDeath</t>
+  </si>
+  <si>
+    <t>143 - 153</t>
+  </si>
+  <si>
+    <t>marraigeBeforeDivorce</t>
+  </si>
+  <si>
+    <t>156 - 166</t>
+  </si>
+  <si>
+    <t>testing.py</t>
+  </si>
+  <si>
+    <t>test_birth_before_death</t>
+  </si>
+  <si>
+    <t>test_marraige_before_divorce</t>
+  </si>
+  <si>
+    <t>007 - 013</t>
+  </si>
+  <si>
+    <t>016 - 021</t>
   </si>
 </sst>
 </file>
@@ -2838,8 +2863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Q21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2853,11 +2878,11 @@
     <col min="8" max="8" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="6" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.5" style="17" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.1640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.6640625" style="17" customWidth="1"/>
     <col min="13" max="13" width="13" style="17" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="1.83203125" style="17" customWidth="1"/>
     <col min="15" max="15" width="10.1640625" style="17" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.5" style="17" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="26.1640625" style="17" customWidth="1"/>
     <col min="17" max="17" width="10.1640625" style="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2970,7 +2995,7 @@
         <v>186</v>
       </c>
       <c r="D4" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="E4">
         <v>20</v>
@@ -2978,8 +3003,32 @@
       <c r="F4">
         <v>20</v>
       </c>
+      <c r="G4">
+        <v>20</v>
+      </c>
+      <c r="H4">
+        <v>20</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>209</v>
+      </c>
       <c r="K4" s="18" t="s">
         <v>207</v>
+      </c>
+      <c r="L4" s="17" t="s">
+        <v>210</v>
+      </c>
+      <c r="M4" s="18" t="s">
+        <v>211</v>
+      </c>
+      <c r="O4" s="18" t="s">
+        <v>214</v>
+      </c>
+      <c r="P4" s="17" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q4" s="18" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.15">
@@ -2993,7 +3042,7 @@
         <v>186</v>
       </c>
       <c r="D5" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="E5">
         <v>35</v>
@@ -3001,8 +3050,32 @@
       <c r="F5">
         <v>30</v>
       </c>
+      <c r="G5">
+        <v>35</v>
+      </c>
+      <c r="H5">
+        <v>30</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>209</v>
+      </c>
       <c r="K5" s="18" t="s">
         <v>207</v>
+      </c>
+      <c r="L5" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="M5" s="18" t="s">
+        <v>213</v>
+      </c>
+      <c r="O5" s="18" t="s">
+        <v>214</v>
+      </c>
+      <c r="P5" s="17" t="s">
+        <v>216</v>
+      </c>
+      <c r="Q5" s="18" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Sprint2 start pair programming
</commit_message>
<xml_diff>
--- a/TeamACNTReport.xlsx
+++ b/TeamACNTReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11110"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/connor/Documents/ssw555/555project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tmcshea44/Documents/CS555/555project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C316DB7-97C9-2C47-9A0C-48E22D7BABCF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B8120D2-B1E5-9E43-9FCF-7B89AB873764}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="13960" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="29040" windowHeight="13940" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -23,10 +23,16 @@
     <sheet name="Sprint4" sheetId="6" r:id="rId8"/>
     <sheet name="Stories" sheetId="11" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -36,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="209">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -692,37 +698,7 @@
     <t>parser.py</t>
   </si>
   <si>
-    <t>Done</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>birthBeforeDeath</t>
-  </si>
-  <si>
-    <t>143 - 153</t>
-  </si>
-  <si>
-    <t>marraigeBeforeDivorce</t>
-  </si>
-  <si>
-    <t>156 - 166</t>
-  </si>
-  <si>
-    <t>testing.py</t>
-  </si>
-  <si>
-    <t>test_birth_before_death</t>
-  </si>
-  <si>
-    <t>test_marraige_before_divorce</t>
-  </si>
-  <si>
-    <t>007 - 013</t>
-  </si>
-  <si>
-    <t>016 - 021</t>
+    <t>Complete</t>
   </si>
 </sst>
 </file>
@@ -2052,7 +2028,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2171,8 +2147,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView topLeftCell="A3" zoomScale="150" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2181,7 +2157,7 @@
     <col min="2" max="2" width="7.6640625" customWidth="1"/>
     <col min="3" max="3" width="28.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.6640625" customWidth="1"/>
-    <col min="5" max="5" width="7.6640625" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
@@ -2215,7 +2191,7 @@
         <v>185</v>
       </c>
       <c r="E2" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
@@ -2232,7 +2208,7 @@
         <v>185</v>
       </c>
       <c r="E3" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
@@ -2249,7 +2225,7 @@
         <v>186</v>
       </c>
       <c r="E4" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
@@ -2266,7 +2242,7 @@
         <v>186</v>
       </c>
       <c r="E5" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
@@ -2283,7 +2259,7 @@
         <v>187</v>
       </c>
       <c r="E6" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
@@ -2300,7 +2276,7 @@
         <v>187</v>
       </c>
       <c r="E7" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
@@ -2317,7 +2293,7 @@
         <v>188</v>
       </c>
       <c r="E8" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
@@ -2334,7 +2310,7 @@
         <v>188</v>
       </c>
       <c r="E9" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
@@ -2347,6 +2323,12 @@
       <c r="C10" t="s">
         <v>77</v>
       </c>
+      <c r="D10" t="s">
+        <v>185</v>
+      </c>
+      <c r="E10" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11">
@@ -2358,6 +2340,12 @@
       <c r="C11" t="s">
         <v>79</v>
       </c>
+      <c r="D11" t="s">
+        <v>185</v>
+      </c>
+      <c r="E11" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12">
@@ -2369,6 +2357,12 @@
       <c r="C12" t="s">
         <v>80</v>
       </c>
+      <c r="D12" t="s">
+        <v>186</v>
+      </c>
+      <c r="E12" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13">
@@ -2380,6 +2374,12 @@
       <c r="C13" t="s">
         <v>81</v>
       </c>
+      <c r="D13" t="s">
+        <v>186</v>
+      </c>
+      <c r="E13" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A14">
@@ -2391,6 +2391,12 @@
       <c r="C14" t="s">
         <v>83</v>
       </c>
+      <c r="D14" t="s">
+        <v>187</v>
+      </c>
+      <c r="E14" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A15">
@@ -2402,6 +2408,12 @@
       <c r="C15" t="s">
         <v>171</v>
       </c>
+      <c r="D15" t="s">
+        <v>187</v>
+      </c>
+      <c r="E15" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16">
@@ -2413,8 +2425,14 @@
       <c r="C16" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D16" t="s">
+        <v>188</v>
+      </c>
+      <c r="E16" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>2</v>
       </c>
@@ -2424,8 +2442,14 @@
       <c r="C17" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D17" t="s">
+        <v>188</v>
+      </c>
+      <c r="E17" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>3</v>
       </c>
@@ -2436,7 +2460,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>3</v>
       </c>
@@ -2447,7 +2471,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>3</v>
       </c>
@@ -2458,7 +2482,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>3</v>
       </c>
@@ -2469,7 +2493,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>3</v>
       </c>
@@ -2480,7 +2504,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>3</v>
       </c>
@@ -2491,7 +2515,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>3</v>
       </c>
@@ -2502,7 +2526,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>3</v>
       </c>
@@ -2513,7 +2537,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>4</v>
       </c>
@@ -2524,7 +2548,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>4</v>
       </c>
@@ -2535,7 +2559,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>4</v>
       </c>
@@ -2546,7 +2570,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>4</v>
       </c>
@@ -2557,7 +2581,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>4</v>
       </c>
@@ -2568,7 +2592,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>4</v>
       </c>
@@ -2579,7 +2603,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>4</v>
       </c>
@@ -2863,8 +2887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Q21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2878,11 +2902,11 @@
     <col min="8" max="8" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="6" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.5" style="17" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.6640625" style="17" customWidth="1"/>
+    <col min="12" max="12" width="19.1640625" style="17" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13" style="17" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="1.83203125" style="17" customWidth="1"/>
     <col min="15" max="15" width="10.1640625" style="17" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="26.1640625" style="17" customWidth="1"/>
+    <col min="16" max="16" width="16.5" style="17" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="10.1640625" style="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2995,7 +3019,7 @@
         <v>186</v>
       </c>
       <c r="D4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E4">
         <v>20</v>
@@ -3003,32 +3027,8 @@
       <c r="F4">
         <v>20</v>
       </c>
-      <c r="G4">
-        <v>20</v>
-      </c>
-      <c r="H4">
-        <v>20</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>209</v>
-      </c>
       <c r="K4" s="18" t="s">
         <v>207</v>
-      </c>
-      <c r="L4" s="17" t="s">
-        <v>210</v>
-      </c>
-      <c r="M4" s="18" t="s">
-        <v>211</v>
-      </c>
-      <c r="O4" s="18" t="s">
-        <v>214</v>
-      </c>
-      <c r="P4" s="17" t="s">
-        <v>215</v>
-      </c>
-      <c r="Q4" s="18" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.15">
@@ -3042,7 +3042,7 @@
         <v>186</v>
       </c>
       <c r="D5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E5">
         <v>35</v>
@@ -3050,32 +3050,8 @@
       <c r="F5">
         <v>30</v>
       </c>
-      <c r="G5">
-        <v>35</v>
-      </c>
-      <c r="H5">
-        <v>30</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>209</v>
-      </c>
       <c r="K5" s="18" t="s">
         <v>207</v>
-      </c>
-      <c r="L5" s="17" t="s">
-        <v>212</v>
-      </c>
-      <c r="M5" s="18" t="s">
-        <v>213</v>
-      </c>
-      <c r="O5" s="18" t="s">
-        <v>214</v>
-      </c>
-      <c r="P5" s="17" t="s">
-        <v>216</v>
-      </c>
-      <c r="Q5" s="18" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.15">
@@ -3142,6 +3118,15 @@
       </c>
       <c r="F8">
         <v>20</v>
+      </c>
+      <c r="G8">
+        <v>15</v>
+      </c>
+      <c r="H8">
+        <v>20</v>
+      </c>
+      <c r="I8" s="6">
+        <v>42416</v>
       </c>
       <c r="K8" s="18" t="s">
         <v>207</v>
@@ -3170,6 +3155,15 @@
       </c>
       <c r="F9">
         <v>30</v>
+      </c>
+      <c r="G9">
+        <v>38</v>
+      </c>
+      <c r="H9">
+        <v>25</v>
+      </c>
+      <c r="I9" s="6">
+        <v>42417</v>
       </c>
       <c r="K9" s="18" t="s">
         <v>207</v>
@@ -3356,8 +3350,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B33" sqref="A10:B33"/>
+    <sheetView topLeftCell="A12" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
update US15 and US16 complete
</commit_message>
<xml_diff>
--- a/TeamACNTReport.xlsx
+++ b/TeamACNTReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tmcshea44/Documents/CS555/555project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{957879AE-72C5-144E-BDC0-10968E9C5150}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21B88F11-CC07-8643-A46C-C8235EE0377B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="251">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -737,34 +737,100 @@
     <t>test_birth_before_marriage</t>
   </si>
   <si>
-    <t>007 - 017</t>
-  </si>
-  <si>
-    <t>019 - 027</t>
-  </si>
-  <si>
-    <t>030 - 036</t>
-  </si>
-  <si>
-    <t>039 - 044</t>
-  </si>
-  <si>
     <t xml:space="preserve">Yes </t>
   </si>
   <si>
     <t>lessThan150</t>
   </si>
   <si>
-    <t>marriageBeforeBirth/divorceAfterBirth</t>
-  </si>
-  <si>
     <t>test_less_than_150_years</t>
   </si>
   <si>
     <t>test_birth_before_marriage_divroce</t>
   </si>
   <si>
-    <t xml:space="preserve">Done </t>
+    <t>Status</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Est Size</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Est Time</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Act Size</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Act Time</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Completed</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>007 - 014</t>
+  </si>
+  <si>
+    <t>016 - 022</t>
+  </si>
+  <si>
+    <t>025-031</t>
+  </si>
+  <si>
+    <t>034- 039</t>
+  </si>
+  <si>
+    <t>marriageBeforeDeath</t>
+  </si>
+  <si>
+    <t>test_marraige_before_death</t>
+  </si>
+  <si>
+    <t>042-045</t>
+  </si>
+  <si>
+    <t>divorceBeforeDeath</t>
+  </si>
+  <si>
+    <t>test_divorce_before_death</t>
+  </si>
+  <si>
+    <t>048-051</t>
+  </si>
+  <si>
+    <t>054-061</t>
+  </si>
+  <si>
+    <t>marriageBeforeBirth</t>
+  </si>
+  <si>
+    <t>063-078</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Complete </t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>familyTreeParser.py</t>
+  </si>
+  <si>
+    <t>maleLastName</t>
+  </si>
+  <si>
+    <t>less15Siblings</t>
+  </si>
+  <si>
+    <t>test_less_than_15_siblings</t>
+  </si>
+  <si>
+    <t>test_male_last_name</t>
   </si>
 </sst>
 </file>
@@ -2226,7 +2292,7 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2714,7 +2780,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D6" zoomScale="150" workbookViewId="0">
+    <sheetView topLeftCell="A18" zoomScale="150" workbookViewId="0">
       <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
@@ -2963,437 +3029,443 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:R21"/>
+  <dimension ref="A1:Q21"/>
   <sheetViews>
     <sheetView zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="O1" sqref="O1:Q1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="7.6640625" customWidth="1"/>
-    <col min="2" max="2" width="32.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="8.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.5" style="17" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="33.83203125" style="17" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.6640625" style="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.5" style="17" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="1.83203125" style="17" customWidth="1"/>
-    <col min="16" max="16" width="10.1640625" style="17" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="31.5" style="17" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.1640625" style="22" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16" style="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.6640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="31.5" style="17" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="10.1640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="31.5" style="17" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.1640625" style="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>12</v>
+        <v>225</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>228</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>17</v>
+        <v>229</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>215</v>
       </c>
       <c r="K1" s="16" t="s">
-        <v>179</v>
+        <v>216</v>
       </c>
       <c r="L1" s="16" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M1" s="16" t="s">
-        <v>215</v>
+        <v>182</v>
       </c>
       <c r="N1" s="16" t="s">
-        <v>216</v>
-      </c>
-      <c r="P1" s="16" t="s">
-        <v>180</v>
-      </c>
-      <c r="Q1" s="16" t="s">
-        <v>182</v>
-      </c>
-      <c r="R1" s="20" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="20"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B2" t="s">
-        <v>157</v>
-      </c>
-      <c r="C2" t="s">
-        <v>184</v>
-      </c>
-      <c r="D2" t="s">
         <v>206</v>
+      </c>
+      <c r="B2">
+        <v>25</v>
+      </c>
+      <c r="C2">
+        <v>30</v>
+      </c>
+      <c r="D2">
+        <f>K2-J2</f>
+        <v>21</v>
       </c>
       <c r="E2">
         <v>25</v>
       </c>
-      <c r="F2">
-        <v>30</v>
-      </c>
-      <c r="G2">
-        <f>N2-M2</f>
-        <v>35</v>
-      </c>
-      <c r="H2">
-        <v>25</v>
-      </c>
-      <c r="I2" s="6" t="s">
+      <c r="F2" s="7" t="s">
         <v>207</v>
       </c>
-      <c r="K2" s="18" t="s">
+      <c r="H2" s="18" t="s">
         <v>205</v>
       </c>
+      <c r="I2" s="18" t="s">
+        <v>213</v>
+      </c>
+      <c r="J2" s="18">
+        <v>161</v>
+      </c>
+      <c r="K2" s="18">
+        <v>182</v>
+      </c>
       <c r="L2" s="18" t="s">
-        <v>213</v>
-      </c>
-      <c r="M2" s="18">
-        <v>160</v>
-      </c>
-      <c r="N2" s="18">
-        <v>195</v>
-      </c>
-      <c r="P2" s="18" t="s">
         <v>210</v>
       </c>
-      <c r="Q2" s="18" t="s">
+      <c r="M2" s="18" t="s">
         <v>219</v>
       </c>
-      <c r="R2" s="23" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="N2" s="23" t="s">
+        <v>231</v>
+      </c>
+      <c r="O2" s="18"/>
+      <c r="P2" s="18"/>
+      <c r="Q2" s="23"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>116</v>
-      </c>
-      <c r="B3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C3" t="s">
-        <v>184</v>
-      </c>
-      <c r="D3" t="s">
         <v>206</v>
       </c>
+      <c r="B3">
+        <v>20</v>
+      </c>
+      <c r="C3">
+        <v>20</v>
+      </c>
+      <c r="D3">
+        <f>K3-J3</f>
+        <v>16</v>
+      </c>
       <c r="E3">
+        <v>15</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="H3" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="I3" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="J3" s="18">
+        <v>187</v>
+      </c>
+      <c r="K3" s="18">
+        <v>203</v>
+      </c>
+      <c r="L3" s="18" t="s">
+        <v>210</v>
+      </c>
+      <c r="M3" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="N3" s="17" t="s">
+        <v>232</v>
+      </c>
+      <c r="O3" s="18"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>206</v>
+      </c>
+      <c r="B4">
         <v>20</v>
       </c>
-      <c r="F3">
+      <c r="C4">
         <v>20</v>
       </c>
-      <c r="G3">
-        <f>N3-M3</f>
-        <v>21</v>
-      </c>
-      <c r="H3">
-        <v>15</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="K3" s="18" t="s">
-        <v>205</v>
-      </c>
-      <c r="L3" s="17" t="s">
-        <v>214</v>
-      </c>
-      <c r="M3" s="18">
-        <v>200</v>
-      </c>
-      <c r="N3" s="18">
-        <v>221</v>
-      </c>
-      <c r="P3" s="18" t="s">
-        <v>210</v>
-      </c>
-      <c r="Q3" s="17" t="s">
-        <v>220</v>
-      </c>
-      <c r="R3" s="22" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A4" t="s">
-        <v>117</v>
-      </c>
-      <c r="B4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C4" t="s">
-        <v>185</v>
-      </c>
-      <c r="D4" t="s">
-        <v>206</v>
+      <c r="D4">
+        <f t="shared" ref="D4:D9" si="0">K4-J4</f>
+        <v>10</v>
       </c>
       <c r="E4">
         <v>20</v>
       </c>
-      <c r="F4">
-        <v>20</v>
-      </c>
-      <c r="G4">
-        <f t="shared" ref="G4:G9" si="0">N4-M4</f>
-        <v>10</v>
-      </c>
-      <c r="H4">
-        <v>20</v>
-      </c>
-      <c r="I4" s="6" t="s">
+      <c r="F4" s="7" t="s">
         <v>207</v>
       </c>
-      <c r="K4" s="18" t="s">
+      <c r="H4" s="18" t="s">
         <v>205</v>
       </c>
-      <c r="L4" s="17" t="s">
+      <c r="I4" s="17" t="s">
         <v>208</v>
       </c>
-      <c r="M4" s="18">
-        <v>225</v>
-      </c>
-      <c r="N4" s="18">
-        <v>235</v>
-      </c>
-      <c r="P4" s="18" t="s">
+      <c r="J4" s="18">
+        <v>207</v>
+      </c>
+      <c r="K4" s="18">
+        <v>217</v>
+      </c>
+      <c r="L4" s="18" t="s">
         <v>210</v>
       </c>
-      <c r="Q4" s="17" t="s">
+      <c r="M4" s="17" t="s">
         <v>211</v>
       </c>
-      <c r="R4" s="21" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="N4" s="18" t="s">
+        <v>233</v>
+      </c>
+      <c r="O4" s="18"/>
+      <c r="Q4" s="21"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>118</v>
-      </c>
-      <c r="B5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C5" t="s">
-        <v>185</v>
-      </c>
-      <c r="D5" t="s">
         <v>206</v>
       </c>
-      <c r="E5">
+      <c r="B5">
         <v>35</v>
       </c>
-      <c r="F5">
+      <c r="C5">
         <v>30</v>
       </c>
-      <c r="G5">
+      <c r="D5">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="H5">
+      <c r="E5">
         <v>30</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="F5" s="7" t="s">
         <v>207</v>
       </c>
-      <c r="K5" s="18" t="s">
+      <c r="H5" s="18" t="s">
         <v>205</v>
       </c>
-      <c r="L5" s="17" t="s">
+      <c r="I5" s="17" t="s">
         <v>209</v>
       </c>
-      <c r="M5" s="18">
+      <c r="J5" s="18">
+        <v>221</v>
+      </c>
+      <c r="K5" s="18">
+        <v>231</v>
+      </c>
+      <c r="L5" s="18" t="s">
+        <v>210</v>
+      </c>
+      <c r="M5" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="N5" s="18" t="s">
+        <v>234</v>
+      </c>
+      <c r="O5" s="18"/>
+      <c r="Q5" s="21"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>204</v>
+      </c>
+      <c r="B6">
+        <v>35</v>
+      </c>
+      <c r="C6">
+        <v>30</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="E6">
+        <v>30</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="H6" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="I6" s="17" t="s">
+        <v>235</v>
+      </c>
+      <c r="J6" s="17">
+        <v>235</v>
+      </c>
+      <c r="K6" s="17">
+        <v>250</v>
+      </c>
+      <c r="L6" s="18" t="s">
+        <v>210</v>
+      </c>
+      <c r="M6" s="17" t="s">
+        <v>236</v>
+      </c>
+      <c r="N6" s="17" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>204</v>
+      </c>
+      <c r="B7">
+        <v>35</v>
+      </c>
+      <c r="C7">
+        <v>30</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="E7">
+        <v>30</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="H7" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="I7" s="17" t="s">
+        <v>238</v>
+      </c>
+      <c r="J7" s="17">
+        <v>254</v>
+      </c>
+      <c r="K7" s="17">
+        <v>269</v>
+      </c>
+      <c r="L7" s="18" t="s">
+        <v>210</v>
+      </c>
+      <c r="M7" s="17" t="s">
         <v>239</v>
       </c>
-      <c r="N5" s="18">
-        <v>249</v>
-      </c>
-      <c r="P5" s="18" t="s">
-        <v>210</v>
-      </c>
-      <c r="Q5" s="17" t="s">
-        <v>212</v>
-      </c>
-      <c r="R5" s="21" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A6" t="s">
-        <v>119</v>
-      </c>
-      <c r="B6" t="s">
-        <v>73</v>
-      </c>
-      <c r="C6" t="s">
-        <v>186</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="N7" s="17" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
         <v>204</v>
       </c>
-      <c r="E6">
-        <v>35</v>
-      </c>
-      <c r="F6">
-        <v>30</v>
-      </c>
-      <c r="G6">
+      <c r="B8">
+        <v>20</v>
+      </c>
+      <c r="C8">
+        <v>20</v>
+      </c>
+      <c r="D8">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K6" s="18" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A7" t="s">
-        <v>120</v>
-      </c>
-      <c r="B7" t="s">
-        <v>74</v>
-      </c>
-      <c r="C7" t="s">
-        <v>186</v>
-      </c>
-      <c r="D7" t="s">
-        <v>204</v>
-      </c>
-      <c r="E7">
-        <v>35</v>
-      </c>
-      <c r="F7">
-        <v>30</v>
-      </c>
-      <c r="G7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K7" s="18" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A8" t="s">
-        <v>121</v>
-      </c>
-      <c r="B8" t="s">
-        <v>75</v>
-      </c>
-      <c r="C8" t="s">
-        <v>187</v>
-      </c>
-      <c r="D8" t="s">
-        <v>206</v>
+        <v>6</v>
       </c>
       <c r="E8">
         <v>20</v>
       </c>
-      <c r="F8">
-        <v>20</v>
-      </c>
-      <c r="G8">
+      <c r="F8" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="H8" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="I8" s="18" t="s">
+        <v>222</v>
+      </c>
+      <c r="J8" s="18">
+        <v>273</v>
+      </c>
+      <c r="K8" s="18">
+        <v>279</v>
+      </c>
+      <c r="L8" s="18" t="s">
+        <v>210</v>
+      </c>
+      <c r="M8" s="18" t="s">
+        <v>223</v>
+      </c>
+      <c r="N8" s="18" t="s">
+        <v>241</v>
+      </c>
+      <c r="O8" s="18"/>
+      <c r="P8" s="18"/>
+      <c r="Q8" s="21"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
+        <v>204</v>
+      </c>
+      <c r="B9">
+        <v>40</v>
+      </c>
+      <c r="C9">
+        <v>30</v>
+      </c>
+      <c r="D9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>20</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>225</v>
-      </c>
-      <c r="K8" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9">
+        <v>25</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="H9" s="18" t="s">
         <v>205</v>
       </c>
-      <c r="L8" s="18" t="s">
-        <v>226</v>
-      </c>
-      <c r="M8" s="18"/>
-      <c r="N8" s="18"/>
-      <c r="P8" s="18" t="s">
+      <c r="I9" s="17" t="s">
+        <v>242</v>
+      </c>
+      <c r="J9" s="17">
+        <v>283</v>
+      </c>
+      <c r="K9" s="17">
+        <v>325</v>
+      </c>
+      <c r="L9" s="18" t="s">
         <v>210</v>
       </c>
-      <c r="Q8" s="18" t="s">
-        <v>228</v>
-      </c>
-      <c r="R8" s="21"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A9" t="s">
-        <v>122</v>
-      </c>
-      <c r="B9" t="s">
-        <v>158</v>
-      </c>
-      <c r="C9" t="s">
-        <v>187</v>
-      </c>
-      <c r="D9" t="s">
-        <v>230</v>
-      </c>
-      <c r="E9">
-        <v>40</v>
-      </c>
-      <c r="F9">
-        <v>30</v>
-      </c>
-      <c r="G9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>25</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="K9" s="18" t="s">
-        <v>205</v>
-      </c>
-      <c r="L9" s="17" t="s">
-        <v>227</v>
-      </c>
-      <c r="P9" s="17" t="s">
-        <v>210</v>
-      </c>
-      <c r="Q9" s="17" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" ht="14" x14ac:dyDescent="0.15">
+      <c r="M9" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="N9" s="17" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="B10"/>
+      <c r="E10">
+        <f>SUM(E2:E9)</f>
+        <v>195</v>
+      </c>
+      <c r="F10" s="7"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+    </row>
+    <row r="14" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="B14" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.15">
       <c r="B15" s="5"/>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="1:18" ht="14" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="B16" s="5" t="s">
         <v>31</v>
       </c>
@@ -3427,18 +3499,24 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:Q9"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3466,8 +3544,30 @@
       <c r="I1" s="10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="J1" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="K1" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="L1" s="16" t="s">
+        <v>215</v>
+      </c>
+      <c r="M1" s="16" t="s">
+        <v>216</v>
+      </c>
+      <c r="N1" s="17"/>
+      <c r="O1" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="P1" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="Q1" s="16" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>123</v>
       </c>
@@ -3481,7 +3581,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>124</v>
       </c>
@@ -3492,7 +3592,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>125</v>
       </c>
@@ -3503,7 +3603,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>126</v>
       </c>
@@ -3514,7 +3614,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>127</v>
       </c>
@@ -3525,7 +3625,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>128</v>
       </c>
@@ -3536,7 +3636,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>129</v>
       </c>
@@ -3546,11 +3646,38 @@
       <c r="C8" t="s">
         <v>187</v>
       </c>
+      <c r="D8" t="s">
+        <v>244</v>
+      </c>
+      <c r="E8">
+        <v>15</v>
+      </c>
+      <c r="F8">
+        <v>15</v>
+      </c>
+      <c r="G8">
+        <v>10</v>
+      </c>
       <c r="H8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+        <v>10</v>
+      </c>
+      <c r="I8" t="s">
+        <v>245</v>
+      </c>
+      <c r="J8" t="s">
+        <v>246</v>
+      </c>
+      <c r="K8" t="s">
+        <v>248</v>
+      </c>
+      <c r="O8" t="s">
+        <v>210</v>
+      </c>
+      <c r="P8" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>130</v>
       </c>
@@ -3559,6 +3686,36 @@
       </c>
       <c r="C9" t="s">
         <v>187</v>
+      </c>
+      <c r="D9" t="s">
+        <v>244</v>
+      </c>
+      <c r="E9">
+        <v>35</v>
+      </c>
+      <c r="F9">
+        <v>40</v>
+      </c>
+      <c r="G9">
+        <v>38</v>
+      </c>
+      <c r="H9">
+        <v>45</v>
+      </c>
+      <c r="I9" t="s">
+        <v>245</v>
+      </c>
+      <c r="J9" t="s">
+        <v>246</v>
+      </c>
+      <c r="K9" t="s">
+        <v>247</v>
+      </c>
+      <c r="O9" t="s">
+        <v>210</v>
+      </c>
+      <c r="P9" t="s">
+        <v>250</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added US10, age_id for finding the age using only an indivID
</commit_message>
<xml_diff>
--- a/TeamACNTReport.xlsx
+++ b/TeamACNTReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22430"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tmcshea44/Documents/CS555/555project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repositories\stevens\555project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21B88F11-CC07-8643-A46C-C8235EE0377B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AACD121A-A664-4F72-BB20-6BD422B924D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-13020" yWindow="5352" windowWidth="13092" windowHeight="11388" tabRatio="500" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -1129,7 +1131,7 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>41065</c:v>
@@ -1200,7 +1202,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2175,16 +2177,16 @@
       <selection sqref="A1:E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -2201,7 +2203,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>184</v>
       </c>
@@ -2218,7 +2220,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>185</v>
       </c>
@@ -2235,7 +2237,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>186</v>
       </c>
@@ -2252,7 +2254,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>187</v>
       </c>
@@ -2269,7 +2271,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D9" s="4" t="s">
         <v>34</v>
       </c>
@@ -2278,7 +2280,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A3:D5">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D5">
     <sortCondition ref="C3:C5"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2295,16 +2297,16 @@
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.1640625" customWidth="1"/>
-    <col min="2" max="2" width="7.6640625" customWidth="1"/>
-    <col min="3" max="3" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" customWidth="1"/>
-    <col min="5" max="5" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.125" customWidth="1"/>
+    <col min="2" max="2" width="7.625" customWidth="1"/>
+    <col min="3" max="3" width="28.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.625" customWidth="1"/>
+    <col min="5" max="5" width="9.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>29</v>
       </c>
@@ -2321,7 +2323,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2338,7 +2340,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2355,7 +2357,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2372,7 +2374,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2389,7 +2391,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2406,7 +2408,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -2423,7 +2425,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -2440,7 +2442,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -2457,7 +2459,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2</v>
       </c>
@@ -2474,7 +2476,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2</v>
       </c>
@@ -2491,7 +2493,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2</v>
       </c>
@@ -2508,7 +2510,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2</v>
       </c>
@@ -2525,7 +2527,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2</v>
       </c>
@@ -2542,7 +2544,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2</v>
       </c>
@@ -2559,7 +2561,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2</v>
       </c>
@@ -2576,7 +2578,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2</v>
       </c>
@@ -2593,7 +2595,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>3</v>
       </c>
@@ -2604,7 +2606,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>3</v>
       </c>
@@ -2615,7 +2617,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>3</v>
       </c>
@@ -2626,7 +2628,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>3</v>
       </c>
@@ -2637,7 +2639,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>3</v>
       </c>
@@ -2648,7 +2650,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>3</v>
       </c>
@@ -2659,7 +2661,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>3</v>
       </c>
@@ -2670,7 +2672,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>3</v>
       </c>
@@ -2681,7 +2683,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>4</v>
       </c>
@@ -2692,7 +2694,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>4</v>
       </c>
@@ -2703,7 +2705,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>4</v>
       </c>
@@ -2714,7 +2716,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>4</v>
       </c>
@@ -2725,7 +2727,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>4</v>
       </c>
@@ -2736,7 +2738,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>4</v>
       </c>
@@ -2747,7 +2749,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>4</v>
       </c>
@@ -2758,7 +2760,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>4</v>
       </c>
@@ -2784,47 +2786,47 @@
       <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="7"/>
+    <col min="1" max="1" width="10.875" style="7"/>
     <col min="2" max="2" width="9.5" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.375" customWidth="1"/>
+    <col min="5" max="5" width="6.875" customWidth="1"/>
     <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>162</v>
       </c>
@@ -2847,7 +2849,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>163</v>
       </c>
@@ -2863,7 +2865,7 @@
       <c r="F15" s="14"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>164</v>
       </c>
@@ -2888,7 +2890,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>165</v>
       </c>
@@ -2913,7 +2915,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>166</v>
       </c>
@@ -2938,7 +2940,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>167</v>
       </c>
@@ -2978,17 +2980,17 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="2"/>
-    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.875" style="2"/>
+    <col min="2" max="2" width="16.625" customWidth="1"/>
     <col min="3" max="3" width="12.5" customWidth="1"/>
-    <col min="4" max="4" width="7.1640625" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="4" max="4" width="7.125" customWidth="1"/>
+    <col min="5" max="5" width="6.875" customWidth="1"/>
     <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3008,7 +3010,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>42408</v>
       </c>
@@ -3031,30 +3033,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Q21"/>
   <sheetViews>
-    <sheetView zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
+    <sheetView topLeftCell="F1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
       <selection activeCell="O1" sqref="O1:Q1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" customWidth="1"/>
+    <col min="1" max="1" width="7.625" customWidth="1"/>
     <col min="2" max="2" width="31" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="8.125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.625" style="6" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16" style="17" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.6640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.625" style="17" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="31.5" style="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="10.1640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="10.125" style="17" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="31.5" style="17" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.1640625" style="22" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.125" style="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>225</v>
       </c>
@@ -3098,7 +3100,7 @@
       <c r="P1" s="16"/>
       <c r="Q1" s="20"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>206</v>
       </c>
@@ -3143,7 +3145,7 @@
       <c r="P2" s="18"/>
       <c r="Q2" s="23"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>206</v>
       </c>
@@ -3186,7 +3188,7 @@
       </c>
       <c r="O3" s="18"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>206</v>
       </c>
@@ -3230,7 +3232,7 @@
       <c r="O4" s="18"/>
       <c r="Q4" s="21"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>206</v>
       </c>
@@ -3274,7 +3276,7 @@
       <c r="O5" s="18"/>
       <c r="Q5" s="21"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>204</v>
       </c>
@@ -3316,7 +3318,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>204</v>
       </c>
@@ -3358,7 +3360,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>204</v>
       </c>
@@ -3403,7 +3405,7 @@
       <c r="P8" s="18"/>
       <c r="Q8" s="21"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>204</v>
       </c>
@@ -3445,7 +3447,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B10"/>
       <c r="E10">
         <f>SUM(E2:E9)</f>
@@ -3456,36 +3458,36 @@
       <c r="I10" s="17"/>
       <c r="J10" s="17"/>
     </row>
-    <row r="14" spans="1:17" ht="14" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B14" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B15" s="5"/>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="1:17" ht="14" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B16" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="2:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="2:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="2:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B20" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="2:2" ht="28" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
         <v>36</v>
       </c>
@@ -3501,22 +3503,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:Q9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17.5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="16" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3567,7 +3569,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>123</v>
       </c>
@@ -3581,7 +3583,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>124</v>
       </c>
@@ -3591,8 +3593,11 @@
       <c r="C3" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="H3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>125</v>
       </c>
@@ -3603,7 +3608,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>126</v>
       </c>
@@ -3614,7 +3619,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>127</v>
       </c>
@@ -3625,7 +3630,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>128</v>
       </c>
@@ -3636,7 +3641,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>129</v>
       </c>
@@ -3677,7 +3682,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>130</v>
       </c>
@@ -3733,9 +3738,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3778,9 +3783,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3819,17 +3824,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView zoomScale="86" zoomScaleNormal="86" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView topLeftCell="A7" zoomScale="86" zoomScaleNormal="86" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>114</v>
       </c>
@@ -3840,7 +3845,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>115</v>
       </c>
@@ -3851,7 +3856,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>116</v>
       </c>
@@ -3862,7 +3867,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>117</v>
       </c>
@@ -3873,7 +3878,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>118</v>
       </c>
@@ -3884,7 +3889,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>119</v>
       </c>
@@ -3895,7 +3900,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>120</v>
       </c>
@@ -3906,7 +3911,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>121</v>
       </c>
@@ -3917,7 +3922,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>122</v>
       </c>
@@ -3928,7 +3933,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>123</v>
       </c>
@@ -3939,7 +3944,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>124</v>
       </c>
@@ -3950,7 +3955,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>125</v>
       </c>
@@ -3961,7 +3966,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>126</v>
       </c>
@@ -3972,7 +3977,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="68" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:3" ht="63" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>127</v>
       </c>
@@ -3983,7 +3988,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>128</v>
       </c>
@@ -3994,7 +3999,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>129</v>
       </c>
@@ -4005,7 +4010,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>130</v>
       </c>
@@ -4016,7 +4021,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>131</v>
       </c>
@@ -4027,7 +4032,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>132</v>
       </c>
@@ -4038,7 +4043,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>133</v>
       </c>
@@ -4049,7 +4054,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>134</v>
       </c>
@@ -4060,7 +4065,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>135</v>
       </c>
@@ -4071,7 +4076,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>136</v>
       </c>
@@ -4082,7 +4087,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>137</v>
       </c>
@@ -4093,7 +4098,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>138</v>
       </c>
@@ -4104,7 +4109,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>139</v>
       </c>
@@ -4115,7 +4120,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="136" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:3" ht="126" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>140</v>
       </c>
@@ -4126,7 +4131,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>141</v>
       </c>
@@ -4137,7 +4142,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>142</v>
       </c>
@@ -4148,7 +4153,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>143</v>
       </c>
@@ -4159,7 +4164,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>144</v>
       </c>
@@ -4170,7 +4175,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>145</v>
       </c>
@@ -4181,7 +4186,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>146</v>
       </c>
@@ -4192,7 +4197,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>147</v>
       </c>
@@ -4203,7 +4208,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>148</v>
       </c>
@@ -4214,7 +4219,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>149</v>
       </c>
@@ -4225,7 +4230,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>150</v>
       </c>
@@ -4236,7 +4241,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>151</v>
       </c>
@@ -4247,7 +4252,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>152</v>
       </c>
@@ -4258,7 +4263,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>153</v>
       </c>
@@ -4269,7 +4274,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>154</v>
       </c>
@@ -4280,7 +4285,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>155</v>
       </c>
@@ -4291,7 +4296,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>156</v>
       </c>

</xml_diff>

<commit_message>
us25 us26 output and tests
</commit_message>
<xml_diff>
--- a/TeamACNTReport.xlsx
+++ b/TeamACNTReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr date1904="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/connor/Documents/ssw555/555project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\555project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E96232F2-585C-4E42-A35A-0CF9EAC62975}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9084C153-A886-469A-9942-9CCD67ECAA67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="860" yWindow="460" windowWidth="26020" windowHeight="15740" tabRatio="500" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3795" yWindow="0" windowWidth="10800" windowHeight="15600" tabRatio="500" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -23,8 +23,16 @@
     <sheet name="Sprint4" sheetId="8" r:id="rId8"/>
     <sheet name="Stories" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="179021" iterateDelta="1E-4"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -33,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="297">
   <si>
     <t>Initials</t>
   </si>
@@ -791,9 +799,6 @@
     <t>All dates should be legitimate dates for the months specified (e.g., 2/30/2015 is not legitimate)</t>
   </si>
   <si>
-    <t>no</t>
-  </si>
-  <si>
     <t>noChildrenMarriage</t>
   </si>
   <si>
@@ -879,16 +884,63 @@
   </si>
   <si>
     <t>* We had some issues with tests getting deleted in merges</t>
+  </si>
+  <si>
+    <t>uniqueFirstName</t>
+  </si>
+  <si>
+    <t>correspondingEntries_individual</t>
+  </si>
+  <si>
+    <t>getPersonAge</t>
+  </si>
+  <si>
+    <t>orderChildren</t>
+  </si>
+  <si>
+    <t>listDeceased</t>
+  </si>
+  <si>
+    <t>listLivingMarried</t>
+  </si>
+  <si>
+    <t>livingSingles</t>
+  </si>
+  <si>
+    <t>multipleBirth</t>
+  </si>
+  <si>
+    <t>test_us25_uniqueFirstName</t>
+  </si>
+  <si>
+    <t>test_us26_correspondingEntries_individual</t>
+  </si>
+  <si>
+    <t>test_us27_getPersonName</t>
+  </si>
+  <si>
+    <t>test_us28_orderChildren</t>
+  </si>
+  <si>
+    <t>212-216</t>
+  </si>
+  <si>
+    <t>230-235</t>
+  </si>
+  <si>
+    <t>238-241</t>
+  </si>
+  <si>
+    <t>220-</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
-    <numFmt numFmtId="166" formatCode="m/d/yyyy"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -955,7 +1007,7 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -2511,17 +2563,17 @@
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.83203125" customWidth="1"/>
+    <col min="1" max="1" width="7.875" customWidth="1"/>
     <col min="2" max="2" width="8" customWidth="1"/>
     <col min="3" max="3" width="7.5" customWidth="1"/>
-    <col min="4" max="4" width="22.33203125" customWidth="1"/>
-    <col min="5" max="5" width="35.1640625" customWidth="1"/>
+    <col min="4" max="4" width="22.375" customWidth="1"/>
+    <col min="5" max="5" width="35.125" customWidth="1"/>
     <col min="6" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2538,7 +2590,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -2555,7 +2607,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -2572,7 +2624,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -2589,7 +2641,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -2606,7 +2658,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D9" s="1" t="s">
         <v>25</v>
       </c>
@@ -2628,17 +2680,17 @@
       <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.1640625" customWidth="1"/>
-    <col min="2" max="2" width="7.6640625" customWidth="1"/>
-    <col min="3" max="3" width="28.6640625" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" customWidth="1"/>
-    <col min="5" max="5" width="9.1640625" customWidth="1"/>
+    <col min="1" max="1" width="5.125" customWidth="1"/>
+    <col min="2" max="2" width="7.625" customWidth="1"/>
+    <col min="3" max="3" width="28.625" customWidth="1"/>
+    <col min="4" max="4" width="6.625" customWidth="1"/>
+    <col min="5" max="5" width="9.125" customWidth="1"/>
     <col min="6" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>27</v>
       </c>
@@ -2655,7 +2707,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2672,7 +2724,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2689,7 +2741,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2706,7 +2758,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2723,7 +2775,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2740,7 +2792,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -2757,7 +2809,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -2774,7 +2826,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -2791,7 +2843,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2</v>
       </c>
@@ -2808,7 +2860,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2</v>
       </c>
@@ -2825,7 +2877,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2</v>
       </c>
@@ -2842,7 +2894,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2</v>
       </c>
@@ -2859,7 +2911,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2</v>
       </c>
@@ -2876,7 +2928,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2</v>
       </c>
@@ -2893,7 +2945,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2</v>
       </c>
@@ -2910,7 +2962,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2</v>
       </c>
@@ -2927,7 +2979,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>3</v>
       </c>
@@ -2944,7 +2996,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>3</v>
       </c>
@@ -2961,7 +3013,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>3</v>
       </c>
@@ -2978,7 +3030,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>3</v>
       </c>
@@ -2995,7 +3047,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>3</v>
       </c>
@@ -3012,7 +3064,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>3</v>
       </c>
@@ -3029,7 +3081,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>3</v>
       </c>
@@ -3046,7 +3098,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>3</v>
       </c>
@@ -3063,7 +3115,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>4</v>
       </c>
@@ -3080,7 +3132,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>4</v>
       </c>
@@ -3097,7 +3149,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>4</v>
       </c>
@@ -3114,7 +3166,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>4</v>
       </c>
@@ -3131,7 +3183,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>4</v>
       </c>
@@ -3148,7 +3200,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>4</v>
       </c>
@@ -3165,7 +3217,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>4</v>
       </c>
@@ -3182,7 +3234,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>4</v>
       </c>
@@ -3213,48 +3265,48 @@
       <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="10.875" style="3" customWidth="1"/>
     <col min="2" max="2" width="9.5" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="3" max="3" width="15.875" customWidth="1"/>
+    <col min="4" max="4" width="12.375" customWidth="1"/>
+    <col min="5" max="5" width="6.875" customWidth="1"/>
     <col min="6" max="6" width="12.5" style="4" customWidth="1"/>
     <col min="7" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
@@ -3277,7 +3329,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>109</v>
       </c>
@@ -3293,7 +3345,7 @@
       <c r="F15" s="8"/>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>110</v>
       </c>
@@ -3318,7 +3370,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>111</v>
       </c>
@@ -3343,7 +3395,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>112</v>
       </c>
@@ -3368,7 +3420,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>113</v>
       </c>
@@ -3408,18 +3460,18 @@
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="16.625" customWidth="1"/>
     <col min="3" max="3" width="12.5" customWidth="1"/>
-    <col min="4" max="4" width="7.1640625" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="4" max="4" width="7.125" customWidth="1"/>
+    <col min="5" max="5" width="6.875" customWidth="1"/>
     <col min="6" max="6" width="12.5" style="4" customWidth="1"/>
     <col min="7" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>103</v>
       </c>
@@ -3439,7 +3491,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>42408</v>
       </c>
@@ -3450,7 +3502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>42423</v>
       </c>
@@ -3472,7 +3524,7 @@
         <v>63.384615384615387</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>42436</v>
       </c>
@@ -3493,7 +3545,7 @@
         <v>87.6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>42457</v>
       </c>
@@ -3529,27 +3581,27 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" customWidth="1"/>
+    <col min="1" max="1" width="7.625" customWidth="1"/>
     <col min="2" max="2" width="31" style="10" customWidth="1"/>
-    <col min="3" max="3" width="7.33203125" customWidth="1"/>
-    <col min="4" max="5" width="8.1640625" customWidth="1"/>
+    <col min="3" max="3" width="7.375" customWidth="1"/>
+    <col min="4" max="5" width="8.125" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
     <col min="7" max="7" width="8.5" customWidth="1"/>
-    <col min="8" max="8" width="9.1640625" customWidth="1"/>
-    <col min="9" max="9" width="21.6640625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="9.125" customWidth="1"/>
+    <col min="9" max="9" width="21.625" style="3" customWidth="1"/>
     <col min="10" max="10" width="17.5" customWidth="1"/>
     <col min="11" max="11" width="16" style="11" customWidth="1"/>
-    <col min="12" max="12" width="17.6640625" style="11" customWidth="1"/>
+    <col min="12" max="12" width="17.625" style="11" customWidth="1"/>
     <col min="13" max="13" width="31.5" style="11" customWidth="1"/>
-    <col min="14" max="15" width="10.1640625" style="11" customWidth="1"/>
+    <col min="14" max="15" width="10.125" style="11" customWidth="1"/>
     <col min="16" max="16" width="31.5" style="11" customWidth="1"/>
-    <col min="17" max="17" width="10.1640625" style="12" customWidth="1"/>
+    <col min="17" max="17" width="10.125" style="12" customWidth="1"/>
     <col min="18" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>31</v>
       </c>
@@ -3593,7 +3645,7 @@
       <c r="P1" s="15"/>
       <c r="Q1" s="16"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>126</v>
       </c>
@@ -3638,7 +3690,7 @@
       <c r="P2" s="17"/>
       <c r="Q2" s="18"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>126</v>
       </c>
@@ -3681,7 +3733,7 @@
       </c>
       <c r="O3" s="17"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>126</v>
       </c>
@@ -3725,7 +3777,7 @@
       <c r="O4" s="17"/>
       <c r="Q4" s="19"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>126</v>
       </c>
@@ -3769,7 +3821,7 @@
       <c r="O5" s="17"/>
       <c r="Q5" s="19"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>126</v>
       </c>
@@ -3811,7 +3863,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>126</v>
       </c>
@@ -3853,7 +3905,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>126</v>
       </c>
@@ -3898,7 +3950,7 @@
       <c r="P8" s="17"/>
       <c r="Q8" s="19"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>126</v>
       </c>
@@ -3940,7 +3992,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="E10">
         <f>SUM(E2:E9)</f>
         <v>195</v>
@@ -3950,35 +4002,35 @@
       <c r="I10" s="11"/>
       <c r="J10" s="11"/>
     </row>
-    <row r="14" spans="1:17" ht="14" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B14" s="20" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B15" s="20"/>
     </row>
-    <row r="16" spans="1:17" ht="14" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B16" s="20" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="17" spans="2:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B17" s="10" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="18" spans="2:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B18" s="10" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="20" spans="2:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B20" s="20" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="21" spans="2:2" ht="28" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B21" s="10" t="s">
         <v>161</v>
       </c>
@@ -3993,26 +4045,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:Q9"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="I1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="P32" sqref="P32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" customWidth="1"/>
+    <col min="2" max="2" width="25.625" customWidth="1"/>
     <col min="3" max="8" width="11" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" customWidth="1"/>
-    <col min="10" max="10" width="18.1640625" customWidth="1"/>
+    <col min="9" max="9" width="11.375" customWidth="1"/>
+    <col min="10" max="10" width="18.125" customWidth="1"/>
     <col min="11" max="11" width="16.5" customWidth="1"/>
     <col min="12" max="12" width="17.5" customWidth="1"/>
     <col min="13" max="13" width="16" customWidth="1"/>
     <col min="14" max="15" width="11" customWidth="1"/>
-    <col min="16" max="16" width="24.1640625" customWidth="1"/>
+    <col min="16" max="16" width="24.125" customWidth="1"/>
     <col min="17" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
@@ -4063,7 +4115,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>49</v>
       </c>
@@ -4113,7 +4165,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>51</v>
       </c>
@@ -4163,7 +4215,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>53</v>
       </c>
@@ -4213,7 +4265,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>55</v>
       </c>
@@ -4263,7 +4315,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>57</v>
       </c>
@@ -4313,7 +4365,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>59</v>
       </c>
@@ -4363,7 +4415,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>61</v>
       </c>
@@ -4413,7 +4465,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>63</v>
       </c>
@@ -4473,17 +4525,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="29.6640625" customWidth="1"/>
+    <col min="2" max="2" width="29.625" customWidth="1"/>
     <col min="3" max="9" width="11" customWidth="1"/>
-    <col min="10" max="10" width="18.83203125" customWidth="1"/>
-    <col min="11" max="11" width="19.6640625" customWidth="1"/>
+    <col min="10" max="10" width="18.875" customWidth="1"/>
+    <col min="11" max="11" width="19.625" customWidth="1"/>
     <col min="12" max="12" width="20.5" customWidth="1"/>
     <col min="13" max="13" width="16.5" customWidth="1"/>
     <col min="14" max="14" width="4" customWidth="1"/>
@@ -4492,7 +4544,7 @@
     <col min="17" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
@@ -4543,7 +4595,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>65</v>
       </c>
@@ -4575,7 +4627,7 @@
         <v>164</v>
       </c>
       <c r="K2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="L2">
         <v>653</v>
@@ -4587,13 +4639,13 @@
         <v>130</v>
       </c>
       <c r="P2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="Q2" s="22" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.15">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>67</v>
       </c>
@@ -4625,7 +4677,7 @@
         <v>164</v>
       </c>
       <c r="K3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="L3">
         <v>674</v>
@@ -4637,13 +4689,13 @@
         <v>130</v>
       </c>
       <c r="P3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="Q3" s="22" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.15">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>69</v>
       </c>
@@ -4675,7 +4727,7 @@
         <v>164</v>
       </c>
       <c r="K4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="L4">
         <v>729</v>
@@ -4687,13 +4739,13 @@
         <v>130</v>
       </c>
       <c r="P4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="Q4" s="22" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.15">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>71</v>
       </c>
@@ -4725,7 +4777,7 @@
         <v>164</v>
       </c>
       <c r="K5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="L5">
         <v>771</v>
@@ -4737,13 +4789,13 @@
         <v>130</v>
       </c>
       <c r="P5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="Q5" s="22" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.15">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>73</v>
       </c>
@@ -4775,7 +4827,7 @@
         <v>164</v>
       </c>
       <c r="K6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="L6">
         <v>782</v>
@@ -4787,13 +4839,13 @@
         <v>130</v>
       </c>
       <c r="P6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="Q6" s="22" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.15">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>75</v>
       </c>
@@ -4825,7 +4877,7 @@
         <v>164</v>
       </c>
       <c r="K7" s="22" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="L7">
         <v>798</v>
@@ -4837,13 +4889,13 @@
         <v>130</v>
       </c>
       <c r="P7" s="22" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q7" s="22" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.15">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>77</v>
       </c>
@@ -4875,7 +4927,7 @@
         <v>164</v>
       </c>
       <c r="K8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="L8">
         <v>813</v>
@@ -4887,13 +4939,13 @@
         <v>130</v>
       </c>
       <c r="P8" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="Q8" s="22" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.15">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>79</v>
       </c>
@@ -4925,7 +4977,7 @@
         <v>164</v>
       </c>
       <c r="K9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="L9">
         <v>831</v>
@@ -4937,13 +4989,13 @@
         <v>130</v>
       </c>
       <c r="P9" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="Q9" s="22" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.15">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="G10">
         <f>SUM(G2:G9)</f>
         <v>144</v>
@@ -4953,29 +5005,29 @@
         <v>225</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B12" s="22" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B13" s="22" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="B13" s="22" t="s">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B14" s="22" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="B14" s="22" t="s">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B16" s="22" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="B16" s="22" t="s">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17" s="22" t="s">
         <v>280</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B17" s="22" t="s">
-        <v>281</v>
       </c>
     </row>
   </sheetData>
@@ -4986,20 +5038,28 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:Q9"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="31" customWidth="1"/>
-    <col min="3" max="1025" width="11" customWidth="1"/>
+    <col min="3" max="9" width="11" customWidth="1"/>
+    <col min="10" max="10" width="18.875" customWidth="1"/>
+    <col min="11" max="11" width="19.625" customWidth="1"/>
+    <col min="12" max="12" width="20.5" customWidth="1"/>
+    <col min="13" max="13" width="16.5" customWidth="1"/>
+    <col min="14" max="14" width="4" customWidth="1"/>
+    <col min="15" max="15" width="11" customWidth="1"/>
+    <col min="16" max="16" width="29.5" customWidth="1"/>
+    <col min="17" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
@@ -5027,8 +5087,30 @@
       <c r="I1" s="13" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="J1" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="K1" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="L1" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="M1" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="N1" s="12"/>
+      <c r="O1" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="P1" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q1" s="16" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>81</v>
       </c>
@@ -5047,11 +5129,38 @@
       <c r="F2">
         <v>20</v>
       </c>
+      <c r="G2">
+        <v>20</v>
+      </c>
+      <c r="H2">
+        <v>15</v>
+      </c>
       <c r="I2" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+        <v>163</v>
+      </c>
+      <c r="J2" t="s">
+        <v>164</v>
+      </c>
+      <c r="K2" t="s">
+        <v>281</v>
+      </c>
+      <c r="L2">
+        <v>851</v>
+      </c>
+      <c r="M2">
+        <v>870</v>
+      </c>
+      <c r="O2" t="s">
+        <v>130</v>
+      </c>
+      <c r="P2" t="s">
+        <v>289</v>
+      </c>
+      <c r="Q2" s="22" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>83</v>
       </c>
@@ -5070,11 +5179,38 @@
       <c r="F3">
         <v>25</v>
       </c>
+      <c r="G3">
+        <v>32</v>
+      </c>
+      <c r="H3">
+        <v>35</v>
+      </c>
       <c r="I3" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+        <v>163</v>
+      </c>
+      <c r="J3" t="s">
+        <v>164</v>
+      </c>
+      <c r="K3" s="22" t="s">
+        <v>282</v>
+      </c>
+      <c r="L3">
+        <v>875</v>
+      </c>
+      <c r="M3">
+        <v>907</v>
+      </c>
+      <c r="O3" t="s">
+        <v>130</v>
+      </c>
+      <c r="P3" t="s">
+        <v>290</v>
+      </c>
+      <c r="Q3" s="22" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>85</v>
       </c>
@@ -5093,11 +5229,38 @@
       <c r="F4">
         <v>10</v>
       </c>
+      <c r="G4">
+        <v>8</v>
+      </c>
+      <c r="H4">
+        <v>8</v>
+      </c>
       <c r="I4" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+        <v>163</v>
+      </c>
+      <c r="J4" t="s">
+        <v>164</v>
+      </c>
+      <c r="K4" t="s">
+        <v>283</v>
+      </c>
+      <c r="L4">
+        <v>912</v>
+      </c>
+      <c r="M4">
+        <v>921</v>
+      </c>
+      <c r="O4" t="s">
+        <v>130</v>
+      </c>
+      <c r="P4" t="s">
+        <v>291</v>
+      </c>
+      <c r="Q4" s="22" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>87</v>
       </c>
@@ -5116,11 +5279,38 @@
       <c r="F5">
         <v>15</v>
       </c>
+      <c r="G5">
+        <v>15</v>
+      </c>
+      <c r="H5">
+        <v>17</v>
+      </c>
       <c r="I5" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+        <v>163</v>
+      </c>
+      <c r="J5" t="s">
+        <v>164</v>
+      </c>
+      <c r="K5" t="s">
+        <v>284</v>
+      </c>
+      <c r="L5">
+        <v>925</v>
+      </c>
+      <c r="M5">
+        <v>939</v>
+      </c>
+      <c r="O5" t="s">
+        <v>130</v>
+      </c>
+      <c r="P5" t="s">
+        <v>292</v>
+      </c>
+      <c r="Q5" s="22" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>89</v>
       </c>
@@ -5139,11 +5329,33 @@
       <c r="F6">
         <v>20</v>
       </c>
+      <c r="G6">
+        <v>6</v>
+      </c>
+      <c r="H6">
+        <v>18</v>
+      </c>
       <c r="I6" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+        <v>163</v>
+      </c>
+      <c r="J6" t="s">
+        <v>164</v>
+      </c>
+      <c r="K6" t="s">
+        <v>285</v>
+      </c>
+      <c r="L6">
+        <v>943</v>
+      </c>
+      <c r="M6">
+        <v>794</v>
+      </c>
+      <c r="O6" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q6" s="22"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>91</v>
       </c>
@@ -5162,11 +5374,34 @@
       <c r="F7">
         <v>20</v>
       </c>
+      <c r="G7">
+        <v>7</v>
+      </c>
+      <c r="H7">
+        <v>16</v>
+      </c>
       <c r="I7" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+        <v>163</v>
+      </c>
+      <c r="J7" t="s">
+        <v>164</v>
+      </c>
+      <c r="K7" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="L7">
+        <v>948</v>
+      </c>
+      <c r="M7">
+        <v>952</v>
+      </c>
+      <c r="O7" t="s">
+        <v>130</v>
+      </c>
+      <c r="P7" s="22"/>
+      <c r="Q7" s="22"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>93</v>
       </c>
@@ -5185,11 +5420,33 @@
       <c r="F8">
         <v>25</v>
       </c>
+      <c r="G8">
+        <v>6</v>
+      </c>
+      <c r="H8">
+        <v>12</v>
+      </c>
       <c r="I8" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+        <v>163</v>
+      </c>
+      <c r="J8" t="s">
+        <v>164</v>
+      </c>
+      <c r="K8" t="s">
+        <v>287</v>
+      </c>
+      <c r="L8">
+        <v>962</v>
+      </c>
+      <c r="M8">
+        <v>971</v>
+      </c>
+      <c r="O8" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q8" s="22"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>95</v>
       </c>
@@ -5208,13 +5465,35 @@
       <c r="F9">
         <v>30</v>
       </c>
+      <c r="G9">
+        <v>18</v>
+      </c>
+      <c r="H9">
+        <v>27</v>
+      </c>
       <c r="I9" t="s">
-        <v>252</v>
-      </c>
+        <v>163</v>
+      </c>
+      <c r="J9" t="s">
+        <v>164</v>
+      </c>
+      <c r="K9" t="s">
+        <v>288</v>
+      </c>
+      <c r="L9">
+        <v>975</v>
+      </c>
+      <c r="M9">
+        <v>994</v>
+      </c>
+      <c r="O9" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q9" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5226,15 +5505,15 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="28.1640625" customWidth="1"/>
+    <col min="2" max="2" width="28.125" customWidth="1"/>
     <col min="3" max="3" width="49.5" style="10" customWidth="1"/>
     <col min="4" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
@@ -5245,7 +5524,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -5256,7 +5535,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -5267,7 +5546,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -5278,7 +5557,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>39</v>
       </c>
@@ -5289,7 +5568,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>41</v>
       </c>
@@ -5300,7 +5579,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -5311,7 +5590,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>45</v>
       </c>
@@ -5322,7 +5601,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>47</v>
       </c>
@@ -5333,7 +5612,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>49</v>
       </c>
@@ -5344,7 +5623,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>51</v>
       </c>
@@ -5355,7 +5634,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>53</v>
       </c>
@@ -5366,7 +5645,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>55</v>
       </c>
@@ -5377,7 +5656,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="68" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:3" ht="63" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>57</v>
       </c>
@@ -5388,7 +5667,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>59</v>
       </c>
@@ -5399,7 +5678,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>61</v>
       </c>
@@ -5410,7 +5689,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>63</v>
       </c>
@@ -5421,7 +5700,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>65</v>
       </c>
@@ -5432,7 +5711,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>67</v>
       </c>
@@ -5443,7 +5722,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>69</v>
       </c>
@@ -5454,7 +5733,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>71</v>
       </c>
@@ -5465,7 +5744,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>73</v>
       </c>
@@ -5476,7 +5755,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>75</v>
       </c>
@@ -5487,7 +5766,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>77</v>
       </c>
@@ -5498,7 +5777,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>79</v>
       </c>
@@ -5509,7 +5788,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>81</v>
       </c>
@@ -5520,7 +5799,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="153" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:3" ht="126" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>83</v>
       </c>
@@ -5531,7 +5810,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>85</v>
       </c>
@@ -5542,7 +5821,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>87</v>
       </c>
@@ -5553,7 +5832,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>89</v>
       </c>
@@ -5564,7 +5843,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>91</v>
       </c>
@@ -5575,7 +5854,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>93</v>
       </c>
@@ -5586,7 +5865,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>95</v>
       </c>
@@ -5597,7 +5876,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>222</v>
       </c>
@@ -5608,7 +5887,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>225</v>
       </c>
@@ -5619,7 +5898,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>228</v>
       </c>
@@ -5630,7 +5909,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>231</v>
       </c>
@@ -5641,7 +5920,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>234</v>
       </c>
@@ -5652,7 +5931,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>237</v>
       </c>
@@ -5663,7 +5942,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>240</v>
       </c>
@@ -5674,7 +5953,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>243</v>
       </c>
@@ -5685,7 +5964,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>246</v>
       </c>
@@ -5696,7 +5975,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>249</v>
       </c>

</xml_diff>

<commit_message>
report updated again, forgot testing line
</commit_message>
<xml_diff>
--- a/TeamACNTReport.xlsx
+++ b/TeamACNTReport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr date1904="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\555project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9084C153-A886-469A-9942-9CCD67ECAA67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58490404-23FD-4A61-8BF5-176E8EA0126E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3795" yWindow="0" windowWidth="10800" windowHeight="15600" tabRatio="500" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3795" yWindow="0" windowWidth="20595" windowHeight="15600" tabRatio="500" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -931,7 +931,7 @@
     <t>238-241</t>
   </si>
   <si>
-    <t>220-</t>
+    <t>220-227</t>
   </si>
 </sst>
 </file>
@@ -5041,7 +5041,7 @@
   <dimension ref="A1:Q9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>